<commit_message>
BF: updated some forms.
</commit_message>
<xml_diff>
--- a/Coverage Survey/Burkina Faso/Oncho/Formulaire Coverage EC TIDC 2020.xlsx
+++ b/Coverage Survey/Burkina Faso/Oncho/Formulaire Coverage EC TIDC 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\Coverage Survey\Burkina Faso\Oncho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0ABA750A-3C10-4FF4-A811-B75A608424CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0E82B62F-6F9C-4C2F-9707-3555B9652D82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="184">
   <si>
     <t>type</t>
   </si>
@@ -300,9 +300,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>Personne_interrogee_</t>
-  </si>
-  <si>
     <t>Chef_de_menage_ou_autre_adulte</t>
   </si>
   <si>
@@ -522,52 +519,61 @@
     <t>Vert</t>
   </si>
   <si>
+    <t>Ménage</t>
+  </si>
+  <si>
+    <t>Lieux de culte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gare routière </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marché  </t>
+  </si>
+  <si>
+    <t>Lieu de travail</t>
+  </si>
+  <si>
+    <t>Autres</t>
+  </si>
+  <si>
+    <t>Ecole</t>
+  </si>
+  <si>
+    <t>Menage</t>
+  </si>
+  <si>
+    <t>Lieux_de_culte</t>
+  </si>
+  <si>
+    <t>Gare-routier</t>
+  </si>
+  <si>
+    <t>Marché</t>
+  </si>
+  <si>
+    <t>Lieu_de_travail</t>
+  </si>
+  <si>
+    <t>Personne_interrogee</t>
+  </si>
+  <si>
+    <t>si enquêté non traité</t>
+  </si>
+  <si>
+    <t>(BF - Novembre 2020) ECT TIDC Oncho - 2. Formulaire Couverture</t>
+  </si>
+  <si>
     <t>bf_ECT_Oncho_2_coverage</t>
   </si>
   <si>
+    <t>select_one Lieux</t>
+  </si>
+  <si>
     <t>${Recu_IVM} = 'Non'</t>
   </si>
   <si>
-    <t>Menage</t>
-  </si>
-  <si>
-    <t>Ménage</t>
-  </si>
-  <si>
-    <t>Lieux_de_culte</t>
-  </si>
-  <si>
-    <t>Lieux de culte</t>
-  </si>
-  <si>
-    <t>Gare-routier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gare routière </t>
-  </si>
-  <si>
-    <t>Marché</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marché  </t>
-  </si>
-  <si>
-    <t>Lieu_de_travail</t>
-  </si>
-  <si>
-    <t>Lieu de travail</t>
-  </si>
-  <si>
-    <t>Ecole</t>
-  </si>
-  <si>
-    <t>Autres</t>
-  </si>
-  <si>
-    <t>select_one Lieux</t>
-  </si>
-  <si>
-    <t>(BF - Novembre 2020) ECT TIDC Oncho - 2. Formulaire Couverture</t>
+    <t>${Repondant} = 'Personne_interrogee'</t>
   </si>
 </sst>
 </file>
@@ -622,7 +628,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,6 +638,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -659,6 +671,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -978,8 +994,8 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1002,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -1011,7 +1027,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>4</v>
@@ -1028,7 +1044,7 @@
         <v>71</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>81</v>
@@ -1042,7 +1058,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>81</v>
@@ -1051,7 +1067,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1062,7 +1078,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>81</v>
@@ -1076,16 +1092,16 @@
         <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1096,7 +1112,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>81</v>
@@ -1113,7 +1129,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>81</v>
@@ -1121,13 +1137,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>81</v>
@@ -1141,16 +1157,16 @@
         <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1158,10 +1174,10 @@
         <v>77</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>143</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>81</v>
@@ -1170,14 +1186,14 @@
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>180</v>
+      <c r="A11" s="12" t="s">
+        <v>181</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>81</v>
@@ -1191,13 +1207,13 @@
         <v>19</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>167</v>
+      <c r="G12" s="12" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1208,7 +1224,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>82</v>
@@ -1225,13 +1241,13 @@
         <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>81</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1239,19 +1255,19 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="D15" t="s">
         <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>148</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>117</v>
+        <v>147</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1259,16 +1275,16 @@
         <v>77</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="D16" t="s">
         <v>81</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1279,30 +1295,30 @@
         <v>22</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>81</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="12" t="s">
         <v>77</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>81</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1313,13 +1329,13 @@
         <v>24</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>81</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1330,7 +1346,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>82</v>
@@ -1347,13 +1363,13 @@
         <v>26</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>81</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1361,50 +1377,57 @@
         <v>77</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>81</v>
       </c>
       <c r="G22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>155</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>81</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="G23" s="1"/>
+        <v>158</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="1"/>
+      <c r="F24" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -1414,7 +1437,7 @@
         <v>27</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>82</v>
@@ -1455,13 +1478,13 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1473,7 +1496,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1554,22 +1577,22 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>92</v>
+      <c r="A9" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>36</v>
@@ -1591,7 +1614,7 @@
         <v>80</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>40</v>
@@ -1602,7 +1625,7 @@
         <v>80</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>41</v>
@@ -1613,7 +1636,7 @@
         <v>80</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>42</v>
@@ -1624,7 +1647,7 @@
         <v>80</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>43</v>
@@ -1635,7 +1658,7 @@
         <v>80</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>44</v>
@@ -1646,7 +1669,7 @@
         <v>80</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>45</v>
@@ -1668,7 +1691,7 @@
         <v>80</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>47</v>
@@ -1701,7 +1724,7 @@
         <v>84</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>48</v>
@@ -1723,7 +1746,7 @@
         <v>84</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>50</v>
@@ -1734,7 +1757,7 @@
         <v>84</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>51</v>
@@ -1756,7 +1779,7 @@
         <v>84</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>53</v>
@@ -1767,7 +1790,7 @@
         <v>86</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>54</v>
@@ -1778,7 +1801,7 @@
         <v>86</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>55</v>
@@ -1811,7 +1834,7 @@
         <v>86</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>58</v>
@@ -1833,7 +1856,7 @@
         <v>86</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>60</v>
@@ -1844,7 +1867,7 @@
         <v>86</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>61</v>
@@ -1855,7 +1878,7 @@
         <v>86</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>62</v>
@@ -1888,7 +1911,7 @@
         <v>88</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>65</v>
@@ -1896,123 +1919,123 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>160</v>
+      </c>
+      <c r="B40" t="s">
         <v>161</v>
       </c>
-      <c r="B40" t="s">
-        <v>162</v>
-      </c>
       <c r="C40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B43" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="C43" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>144</v>
-      </c>
-      <c r="B44" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="C44" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>144</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B50" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C45" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>144</v>
-      </c>
-      <c r="B46" t="s">
-        <v>172</v>
-      </c>
-      <c r="C46" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>144</v>
-      </c>
-      <c r="B47" t="s">
-        <v>174</v>
-      </c>
-      <c r="C47" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>144</v>
-      </c>
-      <c r="B48" t="s">
-        <v>176</v>
-      </c>
-      <c r="C48" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>144</v>
-      </c>
-      <c r="B49" t="s">
-        <v>178</v>
-      </c>
-      <c r="C49" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>144</v>
-      </c>
-      <c r="B50" t="s">
-        <v>179</v>
-      </c>
-      <c r="C50" t="s">
-        <v>179</v>
+      <c r="C50" s="11" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2033,13 +2056,13 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -2055,21 +2078,21 @@
         <v>66</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="C2">
-        <v>20201115</v>
+        <v>20190728</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>